<commit_message>
Added for Program module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LMS_data.xlsx
+++ b/src/test/resources/TestData/LMS_data.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keerthimula/git/Team04_LMS_WebAutomaters/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5167548-846D-5F41-A73E-796C9C39AB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CB760A-59B9-CE4A-AACF-B095A38DD076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="2" xr2:uid="{90208539-8B60-4D51-928E-C6E97A3EC16D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{90208539-8B60-4D51-928E-C6E97A3EC16D}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Program" sheetId="2" r:id="rId3"/>
+    <sheet name="Program" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>password</t>
   </si>
@@ -63,13 +62,31 @@
   </si>
   <si>
     <t>ObjectOrientedAndFunctionalProgram</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>4232#</t>
+  </si>
+  <si>
+    <t>ZSY123 Desc</t>
+  </si>
+  <si>
+    <t>CZX123</t>
+  </si>
+  <si>
+    <t>DAZXS</t>
+  </si>
+  <si>
+    <t>ABC Description123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +105,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,10 +139,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -497,23 +523,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3CAE3B-7221-9F48-8CF1-09B77C36B1EC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D650821-85EF-4949-8C78-543E944494B0}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -525,13 +539,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -543,6 +557,43 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>890364</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logging for Program module. Increased implicit wait to 15 sec
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LMS_data.xlsx
+++ b/src/test/resources/TestData/LMS_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keerthimula/git/Team04_LMS_WebAutomaters/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CB760A-59B9-CE4A-AACF-B095A38DD076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47F5697-0AF0-C847-A48D-D467B512F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{90208539-8B60-4D51-928E-C6E97A3EC16D}"/>
   </bookViews>
@@ -70,16 +70,16 @@
     <t>4232#</t>
   </si>
   <si>
-    <t>ZSY123 Desc</t>
-  </si>
-  <si>
-    <t>CZX123</t>
-  </si>
-  <si>
-    <t>DAZXS</t>
-  </si>
-  <si>
-    <t>ABC Description123</t>
+    <t>greenJavaGreatSelenium</t>
+  </si>
+  <si>
+    <t>allAboutLogic</t>
+  </si>
+  <si>
+    <t>KWAdfd</t>
+  </si>
+  <si>
+    <t>BASicgraet</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,10 +569,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Final updates after clean run
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LMS_data.xlsx
+++ b/src/test/resources/TestData/LMS_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keerthimula/git/Team04_LMS_WebAutomaters_All/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DC3D1A-6CF7-344C-ADE2-CA75480F2888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D540EDE-9D47-C949-B2D7-D34985465608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{90208539-8B60-4D51-928E-C6E97A3EC16D}"/>
   </bookViews>
@@ -70,16 +70,16 @@
     <t>4232#</t>
   </si>
   <si>
-    <t>XCBGTE0yugh234</t>
-  </si>
-  <si>
-    <t>Java6785java</t>
-  </si>
-  <si>
-    <t>javajava</t>
-  </si>
-  <si>
-    <t>AIFeatureCourse4325262</t>
+    <t>Team4kl8Team4Team4</t>
+  </si>
+  <si>
+    <t>javajavkli09Team4</t>
+  </si>
+  <si>
+    <t>JavakjhgflTeam4</t>
+  </si>
+  <si>
+    <t>XkjmnhjkmnhjTeam4</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,10 +569,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -580,12 +580,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>